<commit_message>
Incorporacion de Logica de Anexos Postgres
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Conexion CRGs/databases.xlsx
+++ b/DBA/Reportes BI/2021/Conexion CRGs/databases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personales\Sistemas\Agustin\Reportes BI\2021\Facturación\Informe_Sigehos_CRG\Conexion con DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personales\Sistemas\Agustin\conexion con sigehos\Conexion con DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="178">
   <si>
     <t>database</t>
   </si>
@@ -635,8 +635,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D88" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D87" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D87"/>
   <tableColumns count="4">
     <tableColumn id="1" name="database" dataDxfId="3"/>
     <tableColumn id="5" name="Efector Sigehos" dataDxfId="2"/>
@@ -910,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:XFD82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,111 +1401,111 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="D35" s="1">
-        <v>1644</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1">
-        <v>1855</v>
+        <v>2678</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D37" s="1">
-        <v>2678</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D38" s="1">
-        <v>3118</v>
+        <v>3140</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D39" s="1">
-        <v>3140</v>
+        <v>3031</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D40" s="1">
-        <v>3031</v>
+        <v>3110</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D41" s="1">
-        <v>3110</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D42" s="1">
         <v>-1</v>
@@ -1513,13 +1513,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D43" s="1">
         <v>-1</v>
@@ -1527,13 +1527,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D44" s="1">
         <v>-1</v>
@@ -1541,13 +1541,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D45" s="1">
         <v>-1</v>
@@ -1555,13 +1555,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D46" s="1">
         <v>-1</v>
@@ -1569,13 +1569,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D47" s="1">
         <v>-1</v>
@@ -1583,13 +1583,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D48" s="1">
         <v>-1</v>
@@ -1597,13 +1597,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1">
         <v>-1</v>
@@ -1611,13 +1611,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1">
         <v>-1</v>
@@ -1625,13 +1625,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D51" s="1">
         <v>-1</v>
@@ -1639,13 +1639,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D52" s="1">
         <v>-1</v>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D53" s="1">
         <v>-1</v>
@@ -1667,13 +1667,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D54" s="1">
         <v>-1</v>
@@ -1681,13 +1681,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D55" s="1">
         <v>-1</v>
@@ -1695,13 +1695,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D56" s="1">
         <v>-1</v>
@@ -1709,13 +1709,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D57" s="1">
         <v>-1</v>
@@ -1723,13 +1723,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D58" s="1">
         <v>-1</v>
@@ -1737,13 +1737,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D59" s="1">
         <v>-1</v>
@@ -1751,13 +1751,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D60" s="1">
         <v>-1</v>
@@ -1765,13 +1765,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D61" s="1">
         <v>-1</v>
@@ -1779,13 +1779,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D62" s="1">
         <v>-1</v>
@@ -1793,13 +1793,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D63" s="1">
         <v>-1</v>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D64" s="1">
         <v>-1</v>
@@ -1821,13 +1821,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D65" s="1">
         <v>-1</v>
@@ -1835,13 +1835,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D66" s="1">
         <v>-1</v>
@@ -1849,13 +1849,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D67" s="1">
         <v>-1</v>
@@ -1863,13 +1863,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D68" s="1">
         <v>-1</v>
@@ -1877,13 +1877,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D69" s="1">
         <v>-1</v>
@@ -1891,13 +1891,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D70" s="1">
         <v>-1</v>
@@ -1905,13 +1905,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D71" s="1">
         <v>-1</v>
@@ -1919,13 +1919,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D72" s="1">
         <v>-1</v>
@@ -1933,13 +1933,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D73" s="1">
         <v>-1</v>
@@ -1947,13 +1947,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D74" s="1">
         <v>-1</v>
@@ -1961,13 +1961,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D75" s="1">
         <v>-1</v>
@@ -1975,13 +1975,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D76" s="1">
         <v>-1</v>
@@ -1989,13 +1989,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D77" s="1">
         <v>-1</v>
@@ -2003,13 +2003,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D78" s="1">
         <v>-1</v>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D79" s="1">
         <v>-1</v>
@@ -2031,13 +2031,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D80" s="1">
         <v>-1</v>
@@ -2045,13 +2045,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D81" s="1">
         <v>-1</v>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D82" s="1">
         <v>-1</v>
@@ -2073,13 +2073,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D83" s="1">
         <v>-1</v>
@@ -2087,13 +2087,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D84" s="1">
         <v>-1</v>
@@ -2101,13 +2101,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D85" s="1">
         <v>-1</v>
@@ -2115,13 +2115,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D86" s="1">
         <v>-1</v>
@@ -2129,29 +2129,15 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D87" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D88" s="1">
         <v>-1</v>
       </c>
     </row>

</xml_diff>